<commit_message>
feat: update to v9.15
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-medme-pharmacy-appointment.xlsx
+++ b/site/StructureDefinition-medme-pharmacy-appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="486">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-03T11:11:24-03:00</t>
+    <t>2025-10-30T18:43:23-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -269,7 +269,7 @@
   </si>
   <si>
     <t>app-2:Either start and end are specified, or neither {start.exists() = end.exists()}
-app-3:Only proposed or cancelled appointments can be missing start/end dates {(start.exists() and end.exists()) or (status in ('proposed' | 'cancelled' | 'waitlist'))}app-4:Cancelation reason is only used for appointments that have been cancelled, or no-show {Appointment.cancelationReason.exists() implies (Appointment.status='no-show' or Appointment.status='cancelled')}dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}walkin-no-slot:If appointment type is WALKIN, slot must not be present {appointmentType.coding.where(system = 'https://terminology.hl7.org/CodeSystem/v2-0276' and code = 'WALKIN').exists() or slot.exists()}</t>
+app-3:Only proposed or cancelled appointments can be missing start/end dates {(start.exists() and end.exists()) or (status in ('proposed' | 'cancelled' | 'waitlist'))}app-4:Cancelation reason is only used for appointments that have been cancelled, or no-show {Appointment.cancelationReason.exists() implies (Appointment.status='no-show' or Appointment.status='cancelled')}dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Request</t>
@@ -870,6 +870,10 @@
   </si>
   <si>
     <t>http://terminology.hl7.org/ValueSet/v2-0276</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+walkin-no-slot:If appointment type is WALKIN, slot must not be present {appointmentType.coding.where(system = 'https://terminology.hl7.org/CodeSystem/v2-0276' and code = 'WALKIN').exists() implies slot.empty()}</t>
   </si>
   <si>
     <t>.code</t>
@@ -1250,11 +1254,11 @@
     <t>Appointment.slot</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-slot)
+    <t xml:space="preserve">Reference(Slot|4.0.1)
 </t>
   </si>
   <si>
-    <t>Slot this appointment is booked for</t>
+    <t>The slots that this appointment is filling</t>
   </si>
   <si>
     <t>The slots from the participants' schedules that will be filled by the appointment.</t>
@@ -1429,7 +1433,7 @@
     <t>Appointment.participant.actor</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-patient|https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-healthcare-service|https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-location)
+    <t xml:space="preserve">Reference(Patient|4.0.1|Practitioner|4.0.1|PractitionerRole|4.0.1|RelatedPerson|4.0.1|Device|4.0.1|HealthcareService|4.0.1|Location|4.0.1)
 </t>
   </si>
   <si>
@@ -1842,7 +1846,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="247.83984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="110.0546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -5116,30 +5120,30 @@
         <v>78</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5251,10 +5255,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5368,10 +5372,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5394,19 +5398,19 @@
         <v>90</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>78</v>
@@ -5455,7 +5459,7 @@
         <v>78</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5473,7 +5477,7 @@
         <v>78</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>78</v>
@@ -5482,15 +5486,15 @@
         <v>78</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5602,10 +5606,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5719,10 +5723,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5748,23 +5752,23 @@
         <v>103</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="S34" t="s" s="2">
         <v>78</v>
@@ -5806,7 +5810,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>79</v>
@@ -5824,7 +5828,7 @@
         <v>78</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>78</v>
@@ -5833,15 +5837,15 @@
         <v>78</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5867,13 +5871,13 @@
         <v>176</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5923,7 +5927,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -5941,7 +5945,7 @@
         <v>78</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>78</v>
@@ -5950,15 +5954,15 @@
         <v>78</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5984,14 +5988,14 @@
         <v>109</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>78</v>
@@ -6040,7 +6044,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6058,7 +6062,7 @@
         <v>78</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>78</v>
@@ -6067,15 +6071,15 @@
         <v>78</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6101,14 +6105,14 @@
         <v>176</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>78</v>
@@ -6157,7 +6161,7 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6175,7 +6179,7 @@
         <v>78</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>78</v>
@@ -6184,15 +6188,15 @@
         <v>78</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6215,19 +6219,19 @@
         <v>90</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>78</v>
@@ -6276,7 +6280,7 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6294,7 +6298,7 @@
         <v>78</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>78</v>
@@ -6303,15 +6307,15 @@
         <v>78</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6337,16 +6341,16 @@
         <v>176</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>78</v>
@@ -6395,7 +6399,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6413,7 +6417,7 @@
         <v>78</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>78</v>
@@ -6422,15 +6426,15 @@
         <v>78</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6456,10 +6460,10 @@
         <v>197</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6489,10 +6493,10 @@
         <v>113</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>78</v>
@@ -6510,7 +6514,7 @@
         <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6525,10 +6529,10 @@
         <v>101</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>78</v>
@@ -6537,15 +6541,15 @@
         <v>78</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6568,13 +6572,13 @@
         <v>78</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6625,7 +6629,7 @@
         <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6640,10 +6644,10 @@
         <v>101</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>78</v>
@@ -6657,10 +6661,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6683,16 +6687,16 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6742,7 +6746,7 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6757,27 +6761,27 @@
         <v>101</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>272</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6803,10 +6807,10 @@
         <v>176</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6857,7 +6861,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6875,24 +6879,24 @@
         <v>78</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6915,13 +6919,13 @@
         <v>78</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6972,7 +6976,7 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6987,16 +6991,16 @@
         <v>101</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>78</v>
@@ -7004,10 +7008,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7030,13 +7034,13 @@
         <v>90</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7087,7 +7091,7 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7102,27 +7106,27 @@
         <v>101</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7145,13 +7149,13 @@
         <v>90</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7202,7 +7206,7 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7217,27 +7221,27 @@
         <v>101</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7260,13 +7264,13 @@
         <v>78</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7317,7 +7321,7 @@
         <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7332,13 +7336,13 @@
         <v>101</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>78</v>
@@ -7349,10 +7353,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7375,13 +7379,13 @@
         <v>78</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7432,7 +7436,7 @@
         <v>78</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7450,7 +7454,7 @@
         <v>78</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>78</v>
@@ -7464,10 +7468,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7490,16 +7494,16 @@
         <v>78</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7549,7 +7553,7 @@
         <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -7564,13 +7568,13 @@
         <v>101</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>78</v>
@@ -7581,10 +7585,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7610,13 +7614,13 @@
         <v>176</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7666,7 +7670,7 @@
         <v>78</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7681,27 +7685,27 @@
         <v>101</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7727,10 +7731,10 @@
         <v>176</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7781,7 +7785,7 @@
         <v>78</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -7799,28 +7803,28 @@
         <v>78</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -7839,13 +7843,13 @@
         <v>78</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7896,7 +7900,7 @@
         <v>78</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -7911,10 +7915,10 @@
         <v>101</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>78</v>
@@ -7928,10 +7932,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7954,13 +7958,13 @@
         <v>78</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -8011,7 +8015,7 @@
         <v>78</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>89</v>
@@ -8023,30 +8027,30 @@
         <v>78</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8158,10 +8162,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8275,14 +8279,14 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8304,10 +8308,10 @@
         <v>135</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N56" t="s" s="2">
         <v>163</v>
@@ -8362,7 +8366,7 @@
         <v>78</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>79</v>
@@ -8394,10 +8398,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8423,13 +8427,13 @@
         <v>197</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8458,10 +8462,10 @@
         <v>202</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="Z57" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>78</v>
@@ -8479,7 +8483,7 @@
         <v>78</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>79</v>
@@ -8497,7 +8501,7 @@
         <v>78</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>180</v>
@@ -8506,15 +8510,15 @@
         <v>78</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8537,13 +8541,13 @@
         <v>90</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8594,7 +8598,7 @@
         <v>78</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>79</v>
@@ -8612,24 +8616,24 @@
         <v>78</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8655,10 +8659,10 @@
         <v>109</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8688,10 +8692,10 @@
         <v>191</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>78</v>
@@ -8709,7 +8713,7 @@
         <v>78</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -8727,10 +8731,10 @@
         <v>78</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>78</v>
@@ -8741,10 +8745,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8770,10 +8774,10 @@
         <v>109</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8804,7 +8808,7 @@
       </c>
       <c r="Y60" s="2"/>
       <c r="Z60" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>78</v>
@@ -8822,7 +8826,7 @@
         <v>78</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>89</v>
@@ -8840,24 +8844,24 @@
         <v>78</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8883,10 +8887,10 @@
         <v>226</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8937,7 +8941,7 @@
         <v>78</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -8969,10 +8973,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8998,13 +9002,13 @@
         <v>226</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9054,7 +9058,7 @@
         <v>78</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9069,10 +9073,10 @@
         <v>101</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>78</v>
@@ -9081,7 +9085,7 @@
         <v>78</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update to v9.15 (#5)
</commit_message>
<xml_diff>
--- a/site/StructureDefinition-medme-pharmacy-appointment.xlsx
+++ b/site/StructureDefinition-medme-pharmacy-appointment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="486">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-03T11:11:24-03:00</t>
+    <t>2025-10-30T18:43:23-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -269,7 +269,7 @@
   </si>
   <si>
     <t>app-2:Either start and end are specified, or neither {start.exists() = end.exists()}
-app-3:Only proposed or cancelled appointments can be missing start/end dates {(start.exists() and end.exists()) or (status in ('proposed' | 'cancelled' | 'waitlist'))}app-4:Cancelation reason is only used for appointments that have been cancelled, or no-show {Appointment.cancelationReason.exists() implies (Appointment.status='no-show' or Appointment.status='cancelled')}dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}walkin-no-slot:If appointment type is WALKIN, slot must not be present {appointmentType.coding.where(system = 'https://terminology.hl7.org/CodeSystem/v2-0276' and code = 'WALKIN').exists() or slot.exists()}</t>
+app-3:Only proposed or cancelled appointments can be missing start/end dates {(start.exists() and end.exists()) or (status in ('proposed' | 'cancelled' | 'waitlist'))}app-4:Cancelation reason is only used for appointments that have been cancelled, or no-show {Appointment.cancelationReason.exists() implies (Appointment.status='no-show' or Appointment.status='cancelled')}dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Request</t>
@@ -870,6 +870,10 @@
   </si>
   <si>
     <t>http://terminology.hl7.org/ValueSet/v2-0276</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+walkin-no-slot:If appointment type is WALKIN, slot must not be present {appointmentType.coding.where(system = 'https://terminology.hl7.org/CodeSystem/v2-0276' and code = 'WALKIN').exists() implies slot.empty()}</t>
   </si>
   <si>
     <t>.code</t>
@@ -1250,11 +1254,11 @@
     <t>Appointment.slot</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-slot)
+    <t xml:space="preserve">Reference(Slot|4.0.1)
 </t>
   </si>
   <si>
-    <t>Slot this appointment is booked for</t>
+    <t>The slots that this appointment is filling</t>
   </si>
   <si>
     <t>The slots from the participants' schedules that will be filled by the appointment.</t>
@@ -1429,7 +1433,7 @@
     <t>Appointment.participant.actor</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-patient|https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-healthcare-service|https://fhir.medmehealth.com/pharmacy-services/StructureDefinition/medme-pharmacy-location)
+    <t xml:space="preserve">Reference(Patient|4.0.1|Practitioner|4.0.1|PractitionerRole|4.0.1|RelatedPerson|4.0.1|Device|4.0.1|HealthcareService|4.0.1|Location|4.0.1)
 </t>
   </si>
   <si>
@@ -1842,7 +1846,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="247.83984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="110.0546875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -5116,30 +5120,30 @@
         <v>78</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5251,10 +5255,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5368,10 +5372,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5394,19 +5398,19 @@
         <v>90</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>78</v>
@@ -5455,7 +5459,7 @@
         <v>78</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5473,7 +5477,7 @@
         <v>78</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>78</v>
@@ -5482,15 +5486,15 @@
         <v>78</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5602,10 +5606,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5719,10 +5723,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5748,23 +5752,23 @@
         <v>103</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="S34" t="s" s="2">
         <v>78</v>
@@ -5806,7 +5810,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>79</v>
@@ -5824,7 +5828,7 @@
         <v>78</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>78</v>
@@ -5833,15 +5837,15 @@
         <v>78</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5867,13 +5871,13 @@
         <v>176</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5923,7 +5927,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -5941,7 +5945,7 @@
         <v>78</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>78</v>
@@ -5950,15 +5954,15 @@
         <v>78</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5984,14 +5988,14 @@
         <v>109</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>78</v>
@@ -6040,7 +6044,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6058,7 +6062,7 @@
         <v>78</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>78</v>
@@ -6067,15 +6071,15 @@
         <v>78</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6101,14 +6105,14 @@
         <v>176</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>78</v>
@@ -6157,7 +6161,7 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6175,7 +6179,7 @@
         <v>78</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>78</v>
@@ -6184,15 +6188,15 @@
         <v>78</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6215,19 +6219,19 @@
         <v>90</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>78</v>
@@ -6276,7 +6280,7 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6294,7 +6298,7 @@
         <v>78</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>78</v>
@@ -6303,15 +6307,15 @@
         <v>78</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6337,16 +6341,16 @@
         <v>176</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>78</v>
@@ -6395,7 +6399,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6413,7 +6417,7 @@
         <v>78</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>78</v>
@@ -6422,15 +6426,15 @@
         <v>78</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6456,10 +6460,10 @@
         <v>197</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6489,10 +6493,10 @@
         <v>113</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>78</v>
@@ -6510,7 +6514,7 @@
         <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6525,10 +6529,10 @@
         <v>101</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>78</v>
@@ -6537,15 +6541,15 @@
         <v>78</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6568,13 +6572,13 @@
         <v>78</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6625,7 +6629,7 @@
         <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6640,10 +6644,10 @@
         <v>101</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>78</v>
@@ -6657,10 +6661,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6683,16 +6687,16 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6742,7 +6746,7 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6757,27 +6761,27 @@
         <v>101</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>272</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6803,10 +6807,10 @@
         <v>176</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6857,7 +6861,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -6875,24 +6879,24 @@
         <v>78</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6915,13 +6919,13 @@
         <v>78</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6972,7 +6976,7 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -6987,16 +6991,16 @@
         <v>101</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>78</v>
@@ -7004,10 +7008,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7030,13 +7034,13 @@
         <v>90</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7087,7 +7091,7 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7102,27 +7106,27 @@
         <v>101</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7145,13 +7149,13 @@
         <v>90</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7202,7 +7206,7 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7217,27 +7221,27 @@
         <v>101</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7260,13 +7264,13 @@
         <v>78</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7317,7 +7321,7 @@
         <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7332,13 +7336,13 @@
         <v>101</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>78</v>
@@ -7349,10 +7353,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7375,13 +7379,13 @@
         <v>78</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7432,7 +7436,7 @@
         <v>78</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7450,7 +7454,7 @@
         <v>78</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>78</v>
@@ -7464,10 +7468,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7490,16 +7494,16 @@
         <v>78</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7549,7 +7553,7 @@
         <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -7564,13 +7568,13 @@
         <v>101</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>78</v>
@@ -7581,10 +7585,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7610,13 +7614,13 @@
         <v>176</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7666,7 +7670,7 @@
         <v>78</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7681,27 +7685,27 @@
         <v>101</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7727,10 +7731,10 @@
         <v>176</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7781,7 +7785,7 @@
         <v>78</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -7799,28 +7803,28 @@
         <v>78</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -7839,13 +7843,13 @@
         <v>78</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7896,7 +7900,7 @@
         <v>78</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -7911,10 +7915,10 @@
         <v>101</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>78</v>
@@ -7928,10 +7932,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7954,13 +7958,13 @@
         <v>78</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -8011,7 +8015,7 @@
         <v>78</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>89</v>
@@ -8023,30 +8027,30 @@
         <v>78</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8158,10 +8162,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8275,14 +8279,14 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8304,10 +8308,10 @@
         <v>135</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N56" t="s" s="2">
         <v>163</v>
@@ -8362,7 +8366,7 @@
         <v>78</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>79</v>
@@ -8394,10 +8398,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8423,13 +8427,13 @@
         <v>197</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8458,10 +8462,10 @@
         <v>202</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="Z57" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>78</v>
@@ -8479,7 +8483,7 @@
         <v>78</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>79</v>
@@ -8497,7 +8501,7 @@
         <v>78</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>180</v>
@@ -8506,15 +8510,15 @@
         <v>78</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8537,13 +8541,13 @@
         <v>90</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8594,7 +8598,7 @@
         <v>78</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>79</v>
@@ -8612,24 +8616,24 @@
         <v>78</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8655,10 +8659,10 @@
         <v>109</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8688,10 +8692,10 @@
         <v>191</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>78</v>
@@ -8709,7 +8713,7 @@
         <v>78</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -8727,10 +8731,10 @@
         <v>78</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>78</v>
@@ -8741,10 +8745,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8770,10 +8774,10 @@
         <v>109</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8804,7 +8808,7 @@
       </c>
       <c r="Y60" s="2"/>
       <c r="Z60" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>78</v>
@@ -8822,7 +8826,7 @@
         <v>78</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>89</v>
@@ -8840,24 +8844,24 @@
         <v>78</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8883,10 +8887,10 @@
         <v>226</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8937,7 +8941,7 @@
         <v>78</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -8969,10 +8973,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8998,13 +9002,13 @@
         <v>226</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9054,7 +9058,7 @@
         <v>78</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9069,10 +9073,10 @@
         <v>101</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>78</v>
@@ -9081,7 +9085,7 @@
         <v>78</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>